<commit_message>
- add behavior (working) and main logic (working)
</commit_message>
<xml_diff>
--- a/Карта стенда PSC.xlsx
+++ b/Карта стенда PSC.xlsx
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F61" sqref="F61"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- go to check!!!!
</commit_message>
<xml_diff>
--- a/Карта стенда PSC.xlsx
+++ b/Карта стенда PSC.xlsx
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
- OUT2 requires to fix!
</commit_message>
<xml_diff>
--- a/Карта стенда PSC.xlsx
+++ b/Карта стенда PSC.xlsx
@@ -1,30 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nagin.n\PycharmProjects\psc_web\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\PycharmProjects\psc_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD672CD2-97C7-4D4A-9006-E920A0BB9222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28680" windowHeight="11940"/>
+    <workbookView xWindow="2316" yWindow="1872" windowWidth="16716" windowHeight="9312" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="155">
   <si>
     <t>№</t>
   </si>
@@ -368,9 +376,6 @@
     <t>R2K2</t>
   </si>
   <si>
-    <t>OUT1,2</t>
-  </si>
-  <si>
     <t>КЗ R1</t>
   </si>
   <si>
@@ -486,12 +491,18 @@
   </si>
   <si>
     <t>Обрыв связи с д</t>
+  </si>
+  <si>
+    <t>OUT1</t>
+  </si>
+  <si>
+    <t>OUT2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -872,19 +883,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B56" sqref="B56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -904,7 +915,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -915,7 +926,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -924,7 +935,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -935,7 +946,7 @@
         <v>23</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E3" s="2">
         <v>2</v>
@@ -944,7 +955,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -955,7 +966,7 @@
         <v>24</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E4" s="2">
         <v>3</v>
@@ -964,7 +975,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -975,7 +986,7 @@
         <v>25</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E5" s="2">
         <v>4</v>
@@ -984,7 +995,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -995,7 +1006,7 @@
         <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E6" s="2">
         <v>5</v>
@@ -1004,7 +1015,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1015,7 +1026,7 @@
         <v>27</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E7" s="2">
         <v>6</v>
@@ -1024,7 +1035,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1035,7 +1046,7 @@
         <v>28</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E8" s="2">
         <v>7</v>
@@ -1044,7 +1055,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1055,7 +1066,7 @@
         <v>29</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E9" s="2">
         <v>8</v>
@@ -1064,7 +1075,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1075,7 +1086,7 @@
         <v>30</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E10" s="2">
         <v>9</v>
@@ -1084,7 +1095,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1095,7 +1106,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E11" s="2">
         <v>10</v>
@@ -1104,7 +1115,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1115,7 +1126,7 @@
         <v>32</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E12" s="2">
         <v>11</v>
@@ -1124,7 +1135,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1135,7 +1146,7 @@
         <v>33</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E13" s="2">
         <v>12</v>
@@ -1144,7 +1155,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1155,7 +1166,7 @@
         <v>34</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E14" s="2">
         <v>13</v>
@@ -1164,7 +1175,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -1175,7 +1186,7 @@
         <v>35</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E15" s="2">
         <v>14</v>
@@ -1184,7 +1195,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1195,7 +1206,7 @@
         <v>36</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E16" s="2">
         <v>15</v>
@@ -1204,7 +1215,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -1215,7 +1226,7 @@
         <v>37</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E17" s="2">
         <v>16</v>
@@ -1224,7 +1235,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>0</v>
       </c>
@@ -1244,7 +1255,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>1</v>
       </c>
@@ -1255,7 +1266,7 @@
         <v>54</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E19" s="3">
         <v>17</v>
@@ -1264,7 +1275,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>2</v>
       </c>
@@ -1275,7 +1286,7 @@
         <v>55</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E20" s="3">
         <v>18</v>
@@ -1284,7 +1295,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>3</v>
       </c>
@@ -1295,7 +1306,7 @@
         <v>56</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E21" s="3">
         <v>19</v>
@@ -1304,7 +1315,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>4</v>
       </c>
@@ -1315,7 +1326,7 @@
         <v>57</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E22" s="3">
         <v>20</v>
@@ -1324,7 +1335,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>5</v>
       </c>
@@ -1335,7 +1346,7 @@
         <v>58</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E23" s="3">
         <v>21</v>
@@ -1344,7 +1355,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>6</v>
       </c>
@@ -1355,7 +1366,7 @@
         <v>59</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E24" s="3">
         <v>22</v>
@@ -1364,7 +1375,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>7</v>
       </c>
@@ -1375,7 +1386,7 @@
         <v>60</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E25" s="3">
         <v>23</v>
@@ -1384,7 +1395,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>8</v>
       </c>
@@ -1395,7 +1406,7 @@
         <v>61</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E26" s="3">
         <v>24</v>
@@ -1404,7 +1415,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>9</v>
       </c>
@@ -1415,7 +1426,7 @@
         <v>62</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E27" s="3">
         <v>25</v>
@@ -1424,7 +1435,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>10</v>
       </c>
@@ -1435,7 +1446,7 @@
         <v>63</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E28" s="3">
         <v>26</v>
@@ -1444,7 +1455,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>11</v>
       </c>
@@ -1455,7 +1466,7 @@
         <v>64</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E29" s="3">
         <v>27</v>
@@ -1464,7 +1475,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>12</v>
       </c>
@@ -1475,7 +1486,7 @@
         <v>65</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E30" s="3">
         <v>28</v>
@@ -1484,7 +1495,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>13</v>
       </c>
@@ -1495,7 +1506,7 @@
         <v>66</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E31" s="3">
         <v>29</v>
@@ -1504,7 +1515,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>14</v>
       </c>
@@ -1515,7 +1526,7 @@
         <v>94</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E32" s="3">
         <v>30</v>
@@ -1524,7 +1535,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>15</v>
       </c>
@@ -1535,7 +1546,7 @@
         <v>95</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E33" s="3">
         <v>31</v>
@@ -1544,7 +1555,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>16</v>
       </c>
@@ -1555,7 +1566,7 @@
         <v>96</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E34" s="3">
         <v>32</v>
@@ -1564,7 +1575,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="6" t="s">
         <v>0</v>
       </c>
@@ -1584,7 +1595,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>1</v>
       </c>
@@ -1595,7 +1606,7 @@
         <v>97</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E36" s="2">
         <v>1</v>
@@ -1604,7 +1615,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>2</v>
       </c>
@@ -1612,7 +1623,7 @@
         <v>71</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>103</v>
@@ -1624,7 +1635,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>3</v>
       </c>
@@ -1632,7 +1643,7 @@
         <v>72</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>103</v>
@@ -1644,7 +1655,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>4</v>
       </c>
@@ -1652,7 +1663,7 @@
         <v>73</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>103</v>
@@ -1664,7 +1675,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>5</v>
       </c>
@@ -1672,7 +1683,7 @@
         <v>74</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>103</v>
@@ -1684,7 +1695,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>6</v>
       </c>
@@ -1692,7 +1703,7 @@
         <v>75</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>103</v>
@@ -1704,7 +1715,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>7</v>
       </c>
@@ -1712,7 +1723,7 @@
         <v>76</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>103</v>
@@ -1724,7 +1735,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>8</v>
       </c>
@@ -1744,7 +1755,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>9</v>
       </c>
@@ -1764,7 +1775,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>10</v>
       </c>
@@ -1784,7 +1795,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>11</v>
       </c>
@@ -1804,7 +1815,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>12</v>
       </c>
@@ -1824,7 +1835,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>13</v>
       </c>
@@ -1835,7 +1846,7 @@
         <v>110</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="E48" s="2">
         <v>13</v>
@@ -1844,7 +1855,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>14</v>
       </c>
@@ -1855,7 +1866,7 @@
         <v>111</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>114</v>
+        <v>154</v>
       </c>
       <c r="E49" s="2">
         <v>14</v>
@@ -1864,7 +1875,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>15</v>
       </c>
@@ -1875,7 +1886,7 @@
         <v>112</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="E50" s="2">
         <v>15</v>
@@ -1884,7 +1895,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>16</v>
       </c>
@@ -1895,7 +1906,7 @@
         <v>113</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>114</v>
+        <v>154</v>
       </c>
       <c r="E51" s="2">
         <v>16</v>
@@ -1904,7 +1915,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="6" t="s">
         <v>0</v>
       </c>
@@ -1924,7 +1935,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>1</v>
       </c>
@@ -1932,10 +1943,10 @@
         <v>88</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E53" s="3">
         <v>17</v>
@@ -1944,7 +1955,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>2</v>
       </c>
@@ -1952,10 +1963,10 @@
         <v>89</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E54" s="3">
         <v>18</v>
@@ -1964,7 +1975,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>3</v>
       </c>
@@ -1972,10 +1983,10 @@
         <v>82</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E55" s="3">
         <v>19</v>
@@ -1984,7 +1995,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>4</v>
       </c>
@@ -1992,10 +2003,10 @@
         <v>83</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E56" s="3">
         <v>20</v>
@@ -2004,7 +2015,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>5</v>
       </c>
@@ -2015,7 +2026,7 @@
         <v>102</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E57" s="3">
         <v>21</v>
@@ -2024,7 +2035,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>6</v>
       </c>
@@ -2035,7 +2046,7 @@
         <v>102</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E58" s="3">
         <v>22</v>
@@ -2044,7 +2055,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>7</v>
       </c>
@@ -2055,7 +2066,7 @@
         <v>102</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E59" s="3">
         <v>23</v>
@@ -2064,7 +2075,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>8</v>
       </c>
@@ -2075,7 +2086,7 @@
         <v>102</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E60" s="3">
         <v>24</v>
@@ -2084,99 +2095,99 @@
         <v>101</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>9</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E61" s="3">
         <v>25</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G61" s="7"/>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>10</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E62" s="3">
         <v>26</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>11</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E63" s="3">
         <v>27</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>12</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E64" s="3">
         <v>28</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>13</v>
       </c>
       <c r="B65" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="C65" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="E65" s="3">
         <v>29</v>
@@ -2186,18 +2197,18 @@
         <v>KM20</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>14</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E66" s="3">
         <v>30</v>
@@ -2207,18 +2218,18 @@
         <v>KM21</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>15</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E67" s="3">
         <v>31</v>
@@ -2228,18 +2239,18 @@
         <v>KM22</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>16</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E68" s="3">
         <v>32</v>

</xml_diff>